<commit_message>
fix: change precision in trend
</commit_message>
<xml_diff>
--- a/data_input/REF_WSR.xlsx
+++ b/data_input/REF_WSR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flore\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CBD121-59F8-4742-80F6-FC2D5BDE84F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624D992F-5F8F-4A2B-8AB8-EE852CF3DE17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REF_CONTINENT" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7734" uniqueCount="1423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7734" uniqueCount="1425">
   <si>
     <t>COUNTRY_REGION</t>
   </si>
@@ -4312,6 +4312,12 @@
   </si>
   <si>
     <t>MS Zaandam</t>
+  </si>
+  <si>
+    <t>+,.0f</t>
+  </si>
+  <si>
+    <t>+,.2f</t>
   </si>
 </sst>
 </file>
@@ -4841,7 +4847,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4866,6 +4872,7 @@
     <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5226,12 +5233,12 @@
   </sheetPr>
   <dimension ref="A1:C186"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B11" sqref="B11"/>
       <selection pane="topRight" activeCell="B11" sqref="B11"/>
       <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -46728,7 +46735,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -46908,9 +46915,9 @@
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -47054,8 +47061,8 @@
       <c r="D8" s="5" t="s">
         <v>1404</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>1412</v>
+      <c r="E8" s="10" t="s">
+        <v>1423</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -47071,8 +47078,8 @@
       <c r="D9" s="5" t="s">
         <v>1404</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>1412</v>
+      <c r="E9" s="10" t="s">
+        <v>1423</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -47088,8 +47095,8 @@
       <c r="D10" s="5" t="s">
         <v>1404</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>1412</v>
+      <c r="E10" s="10" t="s">
+        <v>1423</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -47105,8 +47112,8 @@
       <c r="D11" s="5" t="s">
         <v>1404</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>1412</v>
+      <c r="E11" s="10" t="s">
+        <v>1423</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -47122,8 +47129,8 @@
       <c r="D12" s="5" t="s">
         <v>1407</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>1413</v>
+      <c r="E12" s="10" t="s">
+        <v>1424</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -47139,8 +47146,8 @@
       <c r="D13" s="5" t="s">
         <v>1407</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>1413</v>
+      <c r="E13" s="10" t="s">
+        <v>1424</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -47156,8 +47163,8 @@
       <c r="D14" s="5" t="s">
         <v>1406</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>1413</v>
+      <c r="E14" s="10" t="s">
+        <v>1424</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -47173,8 +47180,8 @@
       <c r="D15" s="5" t="s">
         <v>1406</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>1413</v>
+      <c r="E15" s="10" t="s">
+        <v>1424</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -47190,8 +47197,8 @@
       <c r="D16" s="5" t="s">
         <v>1406</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>1413</v>
+      <c r="E16" s="10" t="s">
+        <v>1424</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -47207,8 +47214,8 @@
       <c r="D17" s="5" t="s">
         <v>1406</v>
       </c>
-      <c r="E17" s="5" t="s">
-        <v>1413</v>
+      <c r="E17" s="10" t="s">
+        <v>1424</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
BREAKING CHANGE: data pipeline modification
-add __init__ script to connect to mongo, declare data source and optimise multiples functions
-split covid script world and france > to optimise ressource (not same time of refresh)
-script covid-world : add detailed for US + template for manual input
-script covid-france : add DB_ALL and DB_TREND
-script health-france : new viz
-script eco : add domain for tiles and detailed in stories (021,022,023,024,201BIS,202BIS,203BIS,204BIS) + variation + ml
</commit_message>
<xml_diff>
--- a/data_input/REF_WSR.xlsx
+++ b/data_input/REF_WSR.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flore\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CBD121-59F8-4742-80F6-FC2D5BDE84F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3AEC43D-01A3-48F7-B370-7326AC45DD7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="REF_CONTINENT" sheetId="1" r:id="rId1"/>
-    <sheet name="REF_FRANCE" sheetId="4" r:id="rId2"/>
-    <sheet name="world_countries" sheetId="3" r:id="rId3"/>
-    <sheet name="PARAM_ALL" sheetId="7" r:id="rId4"/>
-    <sheet name="PARAM_TREND" sheetId="5" r:id="rId5"/>
-    <sheet name="PARAM_ENTITIES" sheetId="8" r:id="rId6"/>
+    <sheet name="DATA_INPUT" sheetId="9" r:id="rId1"/>
+    <sheet name="REF_CONTINENT" sheetId="1" r:id="rId2"/>
+    <sheet name="REF_FRANCE" sheetId="4" r:id="rId3"/>
+    <sheet name="world_countries" sheetId="3" r:id="rId4"/>
+    <sheet name="PARAM_ALL" sheetId="7" r:id="rId5"/>
+    <sheet name="PARAM_TREND" sheetId="5" r:id="rId6"/>
+    <sheet name="PARAM_ENTITIES" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">PARAM_ALL!$A$1:$G$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">PARAM_ENTITIES!$A$1:$B$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">PARAM_TREND!$A$1:$E$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">REF_CONTINENT!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">REF_FRANCE!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">world_countries!$A$1:$BQ$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">PARAM_ALL!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">PARAM_ENTITIES!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">PARAM_TREND!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">REF_CONTINENT!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">REF_FRANCE!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">world_countries!$A$1:$BQ$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7734" uniqueCount="1423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7748" uniqueCount="1426">
   <si>
     <t>COUNTRY_REGION</t>
   </si>
@@ -4312,6 +4313,15 @@
   </si>
   <si>
     <t>MS Zaandam</t>
+  </si>
+  <si>
+    <t>Country/Region</t>
+  </si>
+  <si>
+    <t>Province/State</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -4841,7 +4851,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4866,6 +4876,7 @@
     <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5220,18 +5231,1561 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4D81F9A-16FA-4553-9922-0E009ED247E5}">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:F187"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="18.90625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.90625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1423</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1424</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1425</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1394</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1396</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>1397</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="10">
+        <v>20200312</v>
+      </c>
+      <c r="D2" s="5">
+        <v>2313</v>
+      </c>
+      <c r="E2" s="5">
+        <v>196</v>
+      </c>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+    </row>
+    <row r="47" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+    </row>
+    <row r="48" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+    </row>
+    <row r="49" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+    </row>
+    <row r="50" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+    </row>
+    <row r="51" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+    </row>
+    <row r="52" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+    </row>
+    <row r="53" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+    </row>
+    <row r="54" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+    </row>
+    <row r="55" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A55" s="5"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+    </row>
+    <row r="56" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+    </row>
+    <row r="57" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A57" s="5"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+    </row>
+    <row r="58" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A58" s="5"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+    </row>
+    <row r="59" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A59" s="5"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+    </row>
+    <row r="60" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A60" s="5"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+    </row>
+    <row r="61" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A61" s="5"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+    </row>
+    <row r="62" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+    </row>
+    <row r="63" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A63" s="5"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+    </row>
+    <row r="64" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A64" s="5"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+    </row>
+    <row r="65" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A65" s="5"/>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+    </row>
+    <row r="66" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A66" s="5"/>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+    </row>
+    <row r="67" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A67" s="5"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+    </row>
+    <row r="68" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A68" s="5"/>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+    </row>
+    <row r="69" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A69" s="5"/>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+    </row>
+    <row r="70" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A70" s="5"/>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+    </row>
+    <row r="71" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A71" s="5"/>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+    </row>
+    <row r="72" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A72" s="5"/>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+    </row>
+    <row r="73" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A73" s="5"/>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
+    </row>
+    <row r="74" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A74" s="5"/>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
+    </row>
+    <row r="75" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A75" s="5"/>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+    </row>
+    <row r="76" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A76" s="5"/>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+    </row>
+    <row r="77" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A77" s="5"/>
+      <c r="B77" s="5"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="5"/>
+    </row>
+    <row r="78" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A78" s="5"/>
+      <c r="B78" s="5"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
+    </row>
+    <row r="79" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A79" s="5"/>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="5"/>
+    </row>
+    <row r="80" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A80" s="5"/>
+      <c r="B80" s="5"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+    </row>
+    <row r="81" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A81" s="5"/>
+      <c r="B81" s="5"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
+    </row>
+    <row r="82" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A82" s="5"/>
+      <c r="B82" s="5"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="5"/>
+      <c r="F82" s="5"/>
+    </row>
+    <row r="83" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A83" s="5"/>
+      <c r="B83" s="5"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="5"/>
+      <c r="E83" s="5"/>
+      <c r="F83" s="5"/>
+    </row>
+    <row r="84" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A84" s="5"/>
+      <c r="B84" s="5"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="5"/>
+      <c r="F84" s="5"/>
+    </row>
+    <row r="85" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A85" s="5"/>
+      <c r="B85" s="5"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="5"/>
+      <c r="E85" s="5"/>
+      <c r="F85" s="5"/>
+    </row>
+    <row r="86" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A86" s="5"/>
+      <c r="B86" s="5"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+      <c r="E86" s="5"/>
+      <c r="F86" s="5"/>
+    </row>
+    <row r="87" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A87" s="5"/>
+      <c r="B87" s="5"/>
+      <c r="C87" s="5"/>
+      <c r="D87" s="5"/>
+      <c r="E87" s="5"/>
+      <c r="F87" s="5"/>
+    </row>
+    <row r="88" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A88" s="5"/>
+      <c r="B88" s="5"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="5"/>
+      <c r="F88" s="5"/>
+    </row>
+    <row r="89" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A89" s="5"/>
+      <c r="B89" s="5"/>
+      <c r="C89" s="5"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="5"/>
+      <c r="F89" s="5"/>
+    </row>
+    <row r="90" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A90" s="5"/>
+      <c r="B90" s="5"/>
+      <c r="C90" s="5"/>
+      <c r="D90" s="5"/>
+      <c r="E90" s="5"/>
+      <c r="F90" s="5"/>
+    </row>
+    <row r="91" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A91" s="5"/>
+      <c r="B91" s="5"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="5"/>
+      <c r="E91" s="5"/>
+      <c r="F91" s="5"/>
+    </row>
+    <row r="92" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A92" s="5"/>
+      <c r="B92" s="5"/>
+      <c r="C92" s="5"/>
+      <c r="D92" s="5"/>
+      <c r="E92" s="5"/>
+      <c r="F92" s="5"/>
+    </row>
+    <row r="93" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A93" s="5"/>
+      <c r="B93" s="5"/>
+      <c r="C93" s="5"/>
+      <c r="D93" s="5"/>
+      <c r="E93" s="5"/>
+      <c r="F93" s="5"/>
+    </row>
+    <row r="94" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A94" s="5"/>
+      <c r="B94" s="5"/>
+      <c r="C94" s="5"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="5"/>
+      <c r="F94" s="5"/>
+    </row>
+    <row r="95" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A95" s="5"/>
+      <c r="B95" s="5"/>
+      <c r="C95" s="5"/>
+      <c r="D95" s="5"/>
+      <c r="E95" s="5"/>
+      <c r="F95" s="5"/>
+    </row>
+    <row r="96" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A96" s="5"/>
+      <c r="B96" s="5"/>
+      <c r="C96" s="5"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="5"/>
+      <c r="F96" s="5"/>
+    </row>
+    <row r="97" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A97" s="5"/>
+      <c r="B97" s="5"/>
+      <c r="C97" s="5"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="5"/>
+      <c r="F97" s="5"/>
+    </row>
+    <row r="98" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A98" s="5"/>
+      <c r="B98" s="5"/>
+      <c r="C98" s="5"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="5"/>
+    </row>
+    <row r="99" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A99" s="5"/>
+      <c r="B99" s="5"/>
+      <c r="C99" s="5"/>
+      <c r="D99" s="5"/>
+      <c r="E99" s="5"/>
+      <c r="F99" s="5"/>
+    </row>
+    <row r="100" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A100" s="5"/>
+      <c r="B100" s="5"/>
+      <c r="C100" s="5"/>
+      <c r="D100" s="5"/>
+      <c r="E100" s="5"/>
+      <c r="F100" s="5"/>
+    </row>
+    <row r="101" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A101" s="5"/>
+      <c r="B101" s="5"/>
+      <c r="C101" s="5"/>
+      <c r="D101" s="5"/>
+      <c r="E101" s="5"/>
+      <c r="F101" s="5"/>
+    </row>
+    <row r="102" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A102" s="5"/>
+      <c r="B102" s="5"/>
+      <c r="C102" s="5"/>
+      <c r="D102" s="5"/>
+      <c r="E102" s="5"/>
+      <c r="F102" s="5"/>
+    </row>
+    <row r="103" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A103" s="5"/>
+      <c r="B103" s="5"/>
+      <c r="C103" s="5"/>
+      <c r="D103" s="5"/>
+      <c r="E103" s="5"/>
+      <c r="F103" s="5"/>
+    </row>
+    <row r="104" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A104" s="5"/>
+      <c r="B104" s="5"/>
+      <c r="C104" s="5"/>
+      <c r="D104" s="5"/>
+      <c r="E104" s="5"/>
+      <c r="F104" s="5"/>
+    </row>
+    <row r="105" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A105" s="5"/>
+      <c r="B105" s="5"/>
+      <c r="C105" s="5"/>
+      <c r="D105" s="5"/>
+      <c r="E105" s="5"/>
+      <c r="F105" s="5"/>
+    </row>
+    <row r="106" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A106" s="5"/>
+      <c r="B106" s="5"/>
+      <c r="C106" s="5"/>
+      <c r="D106" s="5"/>
+      <c r="E106" s="5"/>
+      <c r="F106" s="5"/>
+    </row>
+    <row r="107" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A107" s="5"/>
+      <c r="B107" s="5"/>
+      <c r="C107" s="5"/>
+      <c r="D107" s="5"/>
+      <c r="E107" s="5"/>
+      <c r="F107" s="5"/>
+    </row>
+    <row r="108" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A108" s="5"/>
+      <c r="B108" s="5"/>
+      <c r="C108" s="5"/>
+      <c r="D108" s="5"/>
+      <c r="E108" s="5"/>
+      <c r="F108" s="5"/>
+    </row>
+    <row r="109" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A109" s="5"/>
+      <c r="B109" s="5"/>
+      <c r="C109" s="5"/>
+      <c r="D109" s="5"/>
+      <c r="E109" s="5"/>
+      <c r="F109" s="5"/>
+    </row>
+    <row r="110" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A110" s="5"/>
+      <c r="B110" s="5"/>
+      <c r="C110" s="5"/>
+      <c r="D110" s="5"/>
+      <c r="E110" s="5"/>
+      <c r="F110" s="5"/>
+    </row>
+    <row r="111" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A111" s="5"/>
+      <c r="B111" s="5"/>
+      <c r="C111" s="5"/>
+      <c r="D111" s="5"/>
+      <c r="E111" s="5"/>
+      <c r="F111" s="5"/>
+    </row>
+    <row r="112" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A112" s="5"/>
+      <c r="B112" s="5"/>
+      <c r="C112" s="5"/>
+      <c r="D112" s="5"/>
+      <c r="E112" s="5"/>
+      <c r="F112" s="5"/>
+    </row>
+    <row r="113" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A113" s="5"/>
+      <c r="B113" s="5"/>
+      <c r="C113" s="5"/>
+      <c r="D113" s="5"/>
+      <c r="E113" s="5"/>
+      <c r="F113" s="5"/>
+    </row>
+    <row r="114" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A114" s="5"/>
+      <c r="B114" s="5"/>
+      <c r="C114" s="5"/>
+      <c r="D114" s="5"/>
+      <c r="E114" s="5"/>
+      <c r="F114" s="5"/>
+    </row>
+    <row r="115" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A115" s="5"/>
+      <c r="B115" s="5"/>
+      <c r="C115" s="5"/>
+      <c r="D115" s="5"/>
+      <c r="E115" s="5"/>
+      <c r="F115" s="5"/>
+    </row>
+    <row r="116" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A116" s="5"/>
+      <c r="B116" s="5"/>
+      <c r="C116" s="5"/>
+      <c r="D116" s="5"/>
+      <c r="E116" s="5"/>
+      <c r="F116" s="5"/>
+    </row>
+    <row r="117" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A117" s="5"/>
+      <c r="B117" s="5"/>
+      <c r="C117" s="5"/>
+      <c r="D117" s="5"/>
+      <c r="E117" s="5"/>
+      <c r="F117" s="5"/>
+    </row>
+    <row r="118" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A118" s="5"/>
+      <c r="B118" s="5"/>
+      <c r="C118" s="5"/>
+      <c r="D118" s="5"/>
+      <c r="E118" s="5"/>
+      <c r="F118" s="5"/>
+    </row>
+    <row r="119" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A119" s="5"/>
+      <c r="B119" s="5"/>
+      <c r="C119" s="5"/>
+      <c r="D119" s="5"/>
+      <c r="E119" s="5"/>
+      <c r="F119" s="5"/>
+    </row>
+    <row r="120" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A120" s="5"/>
+      <c r="B120" s="5"/>
+      <c r="C120" s="5"/>
+      <c r="D120" s="5"/>
+      <c r="E120" s="5"/>
+      <c r="F120" s="5"/>
+    </row>
+    <row r="121" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A121" s="5"/>
+      <c r="B121" s="5"/>
+      <c r="C121" s="5"/>
+      <c r="D121" s="5"/>
+      <c r="E121" s="5"/>
+      <c r="F121" s="5"/>
+    </row>
+    <row r="122" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A122" s="5"/>
+      <c r="B122" s="5"/>
+      <c r="C122" s="5"/>
+      <c r="D122" s="5"/>
+      <c r="E122" s="5"/>
+      <c r="F122" s="5"/>
+    </row>
+    <row r="123" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A123" s="5"/>
+      <c r="B123" s="5"/>
+      <c r="C123" s="5"/>
+      <c r="D123" s="5"/>
+      <c r="E123" s="5"/>
+      <c r="F123" s="5"/>
+    </row>
+    <row r="124" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A124" s="5"/>
+      <c r="B124" s="5"/>
+      <c r="C124" s="5"/>
+      <c r="D124" s="5"/>
+      <c r="E124" s="5"/>
+      <c r="F124" s="5"/>
+    </row>
+    <row r="125" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A125" s="5"/>
+      <c r="B125" s="5"/>
+      <c r="C125" s="5"/>
+      <c r="D125" s="5"/>
+      <c r="E125" s="5"/>
+      <c r="F125" s="5"/>
+    </row>
+    <row r="126" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A126" s="5"/>
+      <c r="B126" s="5"/>
+      <c r="C126" s="5"/>
+      <c r="D126" s="5"/>
+      <c r="E126" s="5"/>
+      <c r="F126" s="5"/>
+    </row>
+    <row r="127" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A127" s="5"/>
+      <c r="B127" s="5"/>
+      <c r="C127" s="5"/>
+      <c r="D127" s="5"/>
+      <c r="E127" s="5"/>
+      <c r="F127" s="5"/>
+    </row>
+    <row r="128" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A128" s="5"/>
+      <c r="B128" s="5"/>
+      <c r="C128" s="5"/>
+      <c r="D128" s="5"/>
+      <c r="E128" s="5"/>
+      <c r="F128" s="5"/>
+    </row>
+    <row r="129" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A129" s="5"/>
+      <c r="B129" s="5"/>
+      <c r="C129" s="5"/>
+      <c r="D129" s="5"/>
+      <c r="E129" s="5"/>
+      <c r="F129" s="5"/>
+    </row>
+    <row r="130" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A130" s="5"/>
+      <c r="B130" s="5"/>
+      <c r="C130" s="5"/>
+      <c r="D130" s="5"/>
+      <c r="E130" s="5"/>
+      <c r="F130" s="5"/>
+    </row>
+    <row r="131" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A131" s="5"/>
+      <c r="B131" s="5"/>
+      <c r="C131" s="5"/>
+      <c r="D131" s="5"/>
+      <c r="E131" s="5"/>
+      <c r="F131" s="5"/>
+    </row>
+    <row r="132" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A132" s="5"/>
+      <c r="B132" s="5"/>
+      <c r="C132" s="5"/>
+      <c r="D132" s="5"/>
+      <c r="E132" s="5"/>
+      <c r="F132" s="5"/>
+    </row>
+    <row r="133" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A133" s="5"/>
+      <c r="B133" s="5"/>
+      <c r="C133" s="5"/>
+      <c r="D133" s="5"/>
+      <c r="E133" s="5"/>
+      <c r="F133" s="5"/>
+    </row>
+    <row r="134" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A134" s="5"/>
+      <c r="B134" s="5"/>
+      <c r="C134" s="5"/>
+      <c r="D134" s="5"/>
+      <c r="E134" s="5"/>
+      <c r="F134" s="5"/>
+    </row>
+    <row r="135" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A135" s="5"/>
+      <c r="B135" s="5"/>
+      <c r="C135" s="5"/>
+      <c r="D135" s="5"/>
+      <c r="E135" s="5"/>
+      <c r="F135" s="5"/>
+    </row>
+    <row r="136" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A136" s="5"/>
+      <c r="B136" s="5"/>
+      <c r="C136" s="5"/>
+      <c r="D136" s="5"/>
+      <c r="E136" s="5"/>
+      <c r="F136" s="5"/>
+    </row>
+    <row r="137" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A137" s="5"/>
+      <c r="B137" s="5"/>
+      <c r="C137" s="5"/>
+      <c r="D137" s="5"/>
+      <c r="E137" s="5"/>
+      <c r="F137" s="5"/>
+    </row>
+    <row r="138" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A138" s="5"/>
+      <c r="B138" s="5"/>
+      <c r="C138" s="5"/>
+      <c r="D138" s="5"/>
+      <c r="E138" s="5"/>
+      <c r="F138" s="5"/>
+    </row>
+    <row r="139" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A139" s="5"/>
+      <c r="B139" s="5"/>
+      <c r="C139" s="5"/>
+      <c r="D139" s="5"/>
+      <c r="E139" s="5"/>
+      <c r="F139" s="5"/>
+    </row>
+    <row r="140" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A140" s="5"/>
+      <c r="B140" s="5"/>
+      <c r="C140" s="5"/>
+      <c r="D140" s="5"/>
+      <c r="E140" s="5"/>
+      <c r="F140" s="5"/>
+    </row>
+    <row r="141" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A141" s="5"/>
+      <c r="B141" s="5"/>
+      <c r="C141" s="5"/>
+      <c r="D141" s="5"/>
+      <c r="E141" s="5"/>
+      <c r="F141" s="5"/>
+    </row>
+    <row r="142" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A142" s="5"/>
+      <c r="B142" s="5"/>
+      <c r="C142" s="5"/>
+      <c r="D142" s="5"/>
+      <c r="E142" s="5"/>
+      <c r="F142" s="5"/>
+    </row>
+    <row r="143" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A143" s="5"/>
+      <c r="B143" s="5"/>
+      <c r="C143" s="5"/>
+      <c r="D143" s="5"/>
+      <c r="E143" s="5"/>
+      <c r="F143" s="5"/>
+    </row>
+    <row r="144" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A144" s="5"/>
+      <c r="B144" s="5"/>
+      <c r="C144" s="5"/>
+      <c r="D144" s="5"/>
+      <c r="E144" s="5"/>
+      <c r="F144" s="5"/>
+    </row>
+    <row r="145" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A145" s="5"/>
+      <c r="B145" s="5"/>
+      <c r="C145" s="5"/>
+      <c r="D145" s="5"/>
+      <c r="E145" s="5"/>
+      <c r="F145" s="5"/>
+    </row>
+    <row r="146" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A146" s="5"/>
+      <c r="B146" s="5"/>
+      <c r="C146" s="5"/>
+      <c r="D146" s="5"/>
+      <c r="E146" s="5"/>
+      <c r="F146" s="5"/>
+    </row>
+    <row r="147" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A147" s="5"/>
+      <c r="B147" s="5"/>
+      <c r="C147" s="5"/>
+      <c r="D147" s="5"/>
+      <c r="E147" s="5"/>
+      <c r="F147" s="5"/>
+    </row>
+    <row r="148" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A148" s="5"/>
+      <c r="B148" s="5"/>
+      <c r="C148" s="5"/>
+      <c r="D148" s="5"/>
+      <c r="E148" s="5"/>
+      <c r="F148" s="5"/>
+    </row>
+    <row r="149" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A149" s="5"/>
+      <c r="B149" s="5"/>
+      <c r="C149" s="5"/>
+      <c r="D149" s="5"/>
+      <c r="E149" s="5"/>
+      <c r="F149" s="5"/>
+    </row>
+    <row r="150" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A150" s="5"/>
+      <c r="B150" s="5"/>
+      <c r="C150" s="5"/>
+      <c r="D150" s="5"/>
+      <c r="E150" s="5"/>
+      <c r="F150" s="5"/>
+    </row>
+    <row r="151" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A151" s="5"/>
+      <c r="B151" s="5"/>
+      <c r="C151" s="5"/>
+      <c r="D151" s="5"/>
+      <c r="E151" s="5"/>
+      <c r="F151" s="5"/>
+    </row>
+    <row r="152" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A152" s="5"/>
+      <c r="B152" s="5"/>
+      <c r="C152" s="5"/>
+      <c r="D152" s="5"/>
+      <c r="E152" s="5"/>
+      <c r="F152" s="5"/>
+    </row>
+    <row r="153" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A153" s="5"/>
+      <c r="B153" s="5"/>
+      <c r="C153" s="5"/>
+      <c r="D153" s="5"/>
+      <c r="E153" s="5"/>
+      <c r="F153" s="5"/>
+    </row>
+    <row r="154" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A154" s="5"/>
+      <c r="B154" s="5"/>
+      <c r="C154" s="5"/>
+      <c r="D154" s="5"/>
+      <c r="E154" s="5"/>
+      <c r="F154" s="5"/>
+    </row>
+    <row r="155" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A155" s="5"/>
+      <c r="B155" s="5"/>
+      <c r="C155" s="5"/>
+      <c r="D155" s="5"/>
+      <c r="E155" s="5"/>
+      <c r="F155" s="5"/>
+    </row>
+    <row r="156" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A156" s="5"/>
+      <c r="B156" s="5"/>
+      <c r="C156" s="5"/>
+      <c r="D156" s="5"/>
+      <c r="E156" s="5"/>
+      <c r="F156" s="5"/>
+    </row>
+    <row r="157" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A157" s="5"/>
+      <c r="B157" s="5"/>
+      <c r="C157" s="5"/>
+      <c r="D157" s="5"/>
+      <c r="E157" s="5"/>
+      <c r="F157" s="5"/>
+    </row>
+    <row r="158" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A158" s="5"/>
+      <c r="B158" s="5"/>
+      <c r="C158" s="5"/>
+      <c r="D158" s="5"/>
+      <c r="E158" s="5"/>
+      <c r="F158" s="5"/>
+    </row>
+    <row r="159" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A159" s="5"/>
+      <c r="B159" s="5"/>
+      <c r="C159" s="5"/>
+      <c r="D159" s="5"/>
+      <c r="E159" s="5"/>
+      <c r="F159" s="5"/>
+    </row>
+    <row r="160" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A160" s="5"/>
+      <c r="B160" s="5"/>
+      <c r="C160" s="5"/>
+      <c r="D160" s="5"/>
+      <c r="E160" s="5"/>
+      <c r="F160" s="5"/>
+    </row>
+    <row r="161" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A161" s="5"/>
+      <c r="B161" s="5"/>
+      <c r="C161" s="5"/>
+      <c r="D161" s="5"/>
+      <c r="E161" s="5"/>
+      <c r="F161" s="5"/>
+    </row>
+    <row r="162" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A162" s="5"/>
+      <c r="B162" s="5"/>
+      <c r="C162" s="5"/>
+      <c r="D162" s="5"/>
+      <c r="E162" s="5"/>
+      <c r="F162" s="5"/>
+    </row>
+    <row r="163" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A163" s="5"/>
+      <c r="B163" s="5"/>
+      <c r="C163" s="5"/>
+      <c r="D163" s="5"/>
+      <c r="E163" s="5"/>
+      <c r="F163" s="5"/>
+    </row>
+    <row r="164" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A164" s="5"/>
+      <c r="B164" s="5"/>
+      <c r="C164" s="5"/>
+      <c r="D164" s="5"/>
+      <c r="E164" s="5"/>
+      <c r="F164" s="5"/>
+    </row>
+    <row r="165" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A165" s="5"/>
+      <c r="B165" s="5"/>
+      <c r="C165" s="5"/>
+      <c r="D165" s="5"/>
+      <c r="E165" s="5"/>
+      <c r="F165" s="5"/>
+    </row>
+    <row r="166" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A166" s="5"/>
+      <c r="B166" s="5"/>
+      <c r="C166" s="5"/>
+      <c r="D166" s="5"/>
+      <c r="E166" s="5"/>
+      <c r="F166" s="5"/>
+    </row>
+    <row r="167" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A167" s="5"/>
+      <c r="B167" s="5"/>
+      <c r="C167" s="5"/>
+      <c r="D167" s="5"/>
+      <c r="E167" s="5"/>
+      <c r="F167" s="5"/>
+    </row>
+    <row r="168" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A168" s="5"/>
+      <c r="B168" s="5"/>
+      <c r="C168" s="5"/>
+      <c r="D168" s="5"/>
+      <c r="E168" s="5"/>
+      <c r="F168" s="5"/>
+    </row>
+    <row r="169" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A169" s="5"/>
+      <c r="B169" s="5"/>
+      <c r="C169" s="5"/>
+      <c r="D169" s="5"/>
+      <c r="E169" s="5"/>
+      <c r="F169" s="5"/>
+    </row>
+    <row r="170" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A170" s="5"/>
+      <c r="B170" s="5"/>
+      <c r="C170" s="5"/>
+      <c r="D170" s="5"/>
+      <c r="E170" s="5"/>
+      <c r="F170" s="5"/>
+    </row>
+    <row r="171" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A171" s="5"/>
+      <c r="B171" s="5"/>
+      <c r="C171" s="5"/>
+      <c r="D171" s="5"/>
+      <c r="E171" s="5"/>
+      <c r="F171" s="5"/>
+    </row>
+    <row r="172" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A172" s="5"/>
+      <c r="B172" s="5"/>
+      <c r="C172" s="5"/>
+      <c r="D172" s="5"/>
+      <c r="E172" s="5"/>
+      <c r="F172" s="5"/>
+    </row>
+    <row r="173" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A173" s="5"/>
+      <c r="B173" s="5"/>
+      <c r="C173" s="5"/>
+      <c r="D173" s="5"/>
+      <c r="E173" s="5"/>
+      <c r="F173" s="5"/>
+    </row>
+    <row r="174" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A174" s="5"/>
+      <c r="B174" s="5"/>
+      <c r="C174" s="5"/>
+      <c r="D174" s="5"/>
+      <c r="E174" s="5"/>
+      <c r="F174" s="5"/>
+    </row>
+    <row r="175" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A175" s="5"/>
+      <c r="B175" s="5"/>
+      <c r="C175" s="5"/>
+      <c r="D175" s="5"/>
+      <c r="E175" s="5"/>
+      <c r="F175" s="5"/>
+    </row>
+    <row r="176" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A176" s="5"/>
+      <c r="B176" s="5"/>
+      <c r="C176" s="5"/>
+      <c r="D176" s="5"/>
+      <c r="E176" s="5"/>
+      <c r="F176" s="5"/>
+    </row>
+    <row r="177" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A177" s="5"/>
+      <c r="B177" s="5"/>
+      <c r="C177" s="5"/>
+      <c r="D177" s="5"/>
+      <c r="E177" s="5"/>
+      <c r="F177" s="5"/>
+    </row>
+    <row r="178" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A178" s="5"/>
+      <c r="B178" s="5"/>
+      <c r="C178" s="5"/>
+      <c r="D178" s="5"/>
+      <c r="E178" s="5"/>
+      <c r="F178" s="5"/>
+    </row>
+    <row r="179" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A179" s="5"/>
+      <c r="B179" s="5"/>
+      <c r="C179" s="5"/>
+      <c r="D179" s="5"/>
+      <c r="E179" s="5"/>
+      <c r="F179" s="5"/>
+    </row>
+    <row r="180" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A180" s="5"/>
+      <c r="B180" s="5"/>
+      <c r="C180" s="5"/>
+      <c r="D180" s="5"/>
+      <c r="E180" s="5"/>
+      <c r="F180" s="5"/>
+    </row>
+    <row r="181" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A181" s="5"/>
+      <c r="B181" s="5"/>
+      <c r="C181" s="5"/>
+      <c r="D181" s="5"/>
+      <c r="E181" s="5"/>
+      <c r="F181" s="5"/>
+    </row>
+    <row r="182" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A182" s="5"/>
+      <c r="B182" s="5"/>
+      <c r="C182" s="5"/>
+      <c r="D182" s="5"/>
+      <c r="E182" s="5"/>
+      <c r="F182" s="5"/>
+    </row>
+    <row r="183" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A183" s="5"/>
+      <c r="B183" s="5"/>
+      <c r="C183" s="5"/>
+      <c r="D183" s="5"/>
+      <c r="E183" s="5"/>
+      <c r="F183" s="5"/>
+    </row>
+    <row r="184" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A184" s="5"/>
+      <c r="B184" s="5"/>
+      <c r="C184" s="5"/>
+      <c r="D184" s="5"/>
+      <c r="E184" s="5"/>
+      <c r="F184" s="5"/>
+    </row>
+    <row r="185" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A185" s="5"/>
+      <c r="B185" s="5"/>
+      <c r="C185" s="5"/>
+      <c r="D185" s="5"/>
+      <c r="E185" s="5"/>
+      <c r="F185" s="5"/>
+    </row>
+    <row r="186" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A186" s="5"/>
+      <c r="B186" s="5"/>
+      <c r="C186" s="5"/>
+      <c r="D186" s="5"/>
+      <c r="E186" s="5"/>
+      <c r="F186" s="5"/>
+    </row>
+    <row r="187" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A187" s="5"/>
+      <c r="B187" s="5"/>
+      <c r="C187" s="5"/>
+      <c r="D187" s="5"/>
+      <c r="E187" s="5"/>
+      <c r="F187" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:C186"/>
+  <dimension ref="A1:C188"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B174" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B11" sqref="B11"/>
       <selection pane="topRight" activeCell="B11" sqref="B11"/>
       <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="B188" sqref="B188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -6993,304 +8547,326 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
-        <v>141</v>
+        <v>1072</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C160" s="5" t="s">
-        <v>141</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B161" s="5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C161" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B163" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B165" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C165" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
-        <v>177</v>
+        <v>146</v>
       </c>
       <c r="B166" s="5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>177</v>
+        <v>146</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
-        <v>147</v>
+        <v>177</v>
       </c>
       <c r="B167" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>219</v>
+        <v>177</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B168" s="5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>148</v>
+        <v>219</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B169" s="5" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C169" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
-        <v>178</v>
+        <v>149</v>
       </c>
       <c r="B170" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C170" s="5" t="s">
-        <v>178</v>
+        <v>149</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
-        <v>150</v>
+        <v>178</v>
       </c>
       <c r="B171" s="5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C171" s="5" t="s">
-        <v>150</v>
+        <v>178</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B172" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C172" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B173" s="5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C173" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B174" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C174" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="B175" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C175" s="5" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
-        <v>154</v>
+        <v>173</v>
       </c>
       <c r="B176" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C176" s="5" t="s">
-        <v>154</v>
+        <v>173</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B177" s="5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C177" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B178" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C178" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B179" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C179" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B180" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C180" s="5" t="s">
-        <v>220</v>
+        <v>157</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B181" s="5" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C181" s="5" t="s">
-        <v>159</v>
+        <v>220</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B182" s="5" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C182" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B183" s="5" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C183" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="5" t="s">
-        <v>1029</v>
+        <v>161</v>
       </c>
       <c r="B184" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C184" s="5" t="s">
-        <v>210</v>
+        <v>161</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="5" t="s">
-        <v>162</v>
+        <v>1029</v>
       </c>
       <c r="B185" s="5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C185" s="5" t="s">
-        <v>162</v>
+        <v>210</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B186" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C186" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" s="5" t="s">
         <v>169</v>
+      </c>
+      <c r="B187" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C187" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" s="5" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B188" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C188" s="5" t="s">
+        <v>1056</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1" xr:uid="{3CBD59A3-86DD-499F-804D-BF7954CAE9A8}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C186">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C187">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
@@ -7299,7 +8875,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{196708D6-1758-49BE-89C9-21E8EA0F5DDC}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -8448,7 +10024,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BQ204"/>
   <sheetViews>
@@ -46719,7 +48295,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8431BF20-F1A5-4EF8-8C24-6266CE091EE3}">
   <sheetPr>
     <tabColor theme="0" tint="-0.14999847407452621"/>
@@ -46901,7 +48477,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{482127E3-95D3-4BB6-B407-4DD8849DDEDC}">
   <sheetPr>
     <tabColor theme="0" tint="-0.14999847407452621"/>
@@ -47244,7 +48820,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A6DFFE9-5C8A-4067-A6FE-248DEB2D7D48}">
   <sheetPr>
     <tabColor theme="0" tint="-0.14999847407452621"/>

</xml_diff>

<commit_message>
feat: france map chart
add France geojson, script python, update name in REF_WSR
</commit_message>
<xml_diff>
--- a/data_input/REF_WSR.xlsx
+++ b/data_input/REF_WSR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flore\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F65DF10-4604-408B-890C-FB4DAD076177}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B495ECE-6B65-4BC0-A39B-869E6E34D305}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA_INPUT" sheetId="9" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">PARAM_ENTITIES!$A$1:$B$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">PARAM_TREND!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">REF_CONTINENT!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">REF_FRANCE!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">REF_FRANCE!$A$1:$C$102</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">world_countries!$A$1:$BQ$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -3910,9 +3910,6 @@
     <t>Côte-d'Or</t>
   </si>
   <si>
-    <t>Côtes d'Armor</t>
-  </si>
-  <si>
     <t>Creuse</t>
   </si>
   <si>
@@ -4117,9 +4114,6 @@
     <t>Val-de-Marne</t>
   </si>
   <si>
-    <t>Val-D'Oise</t>
-  </si>
-  <si>
     <t>Guadeloupe</t>
   </si>
   <si>
@@ -4177,9 +4171,6 @@
     <t>Pays de la Loire</t>
   </si>
   <si>
-    <t>Ile-de-France</t>
-  </si>
-  <si>
     <t>Vendée</t>
   </si>
   <si>
@@ -4328,6 +4319,15 @@
   </si>
   <si>
     <t>+,.2f</t>
+  </si>
+  <si>
+    <t>Côtes-d'Armor</t>
+  </si>
+  <si>
+    <t>Val-d'Oise</t>
+  </si>
+  <si>
+    <t>Île-de-France</t>
   </si>
 </sst>
 </file>
@@ -5258,22 +5258,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>1423</v>
+        <v>1420</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1424</v>
+        <v>1421</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1425</v>
+        <v>1422</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>1391</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1393</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>1394</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>1396</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>1397</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -7124,13 +7124,13 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>1421</v>
+        <v>1418</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>1421</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -8147,13 +8147,13 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>1422</v>
+        <v>1419</v>
       </c>
       <c r="B123" s="5" t="s">
         <v>1263</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>1422</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -8884,14 +8884,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{196708D6-1758-49BE-89C9-21E8EA0F5DDC}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C77" sqref="C77:C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -8904,115 +8904,115 @@
   <sheetData>
     <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1381</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1382</v>
+        <v>1379</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>1264</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>1364</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1383</v>
+        <v>1380</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>1265</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>1365</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>1384</v>
+        <v>1381</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>1266</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>1364</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>1385</v>
+        <v>1382</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>1267</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>1366</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>1386</v>
+        <v>1383</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>1268</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>1366</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>1387</v>
+        <v>1384</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>1269</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>1366</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>1388</v>
+        <v>1385</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>1270</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>1364</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>1389</v>
+        <v>1386</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>1271</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>1367</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>1390</v>
+        <v>1387</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>1272</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>1368</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -9020,10 +9020,10 @@
         <v>1273</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>1367</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -9031,10 +9031,10 @@
         <v>1274</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>1368</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -9042,10 +9042,10 @@
         <v>1275</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>1368</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -9053,10 +9053,10 @@
         <v>1276</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>1366</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -9064,10 +9064,10 @@
         <v>1277</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>1369</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -9075,10 +9075,10 @@
         <v>1278</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>1364</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -9086,10 +9086,10 @@
         <v>1279</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -9097,10 +9097,10 @@
         <v>1280</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -9108,10 +9108,10 @@
         <v>1281</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>1371</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -9119,10 +9119,10 @@
         <v>1282</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>1283</v>
       </c>
@@ -9130,10 +9130,10 @@
         <v>1284</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>1372</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>1285</v>
       </c>
@@ -9141,10 +9141,10 @@
         <v>1286</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>1372</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -9152,590 +9152,590 @@
         <v>1287</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>1373</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>22</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>1288</v>
+        <v>1425</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>1374</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>23</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>24</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>25</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>1373</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>26</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>1364</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>27</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>1369</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>28</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>1371</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>29</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>1374</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>30</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>1368</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>31</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>1368</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>32</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>1368</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>33</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>34</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>1368</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>35</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>1374</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>36</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>1371</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>37</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>1371</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>38</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>1364</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>39</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>1373</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>40</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>41</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>1371</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>42</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>1364</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>43</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>1364</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>44</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>45</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>1371</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>46</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>1368</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>47</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>48</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>1368</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>49</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>50</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>1369</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>51</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>1367</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>52</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>1367</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>53</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>54</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>1367</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>55</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>1367</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>56</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>1374</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>57</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>1367</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>58</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>1373</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>59</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>1365</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>60</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>1365</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>61</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>1369</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>62</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>1365</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>63</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>1364</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>64</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>65</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>1368</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>66</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>1368</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>67</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>1367</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>68</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>1367</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>69</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>1364</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>70</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>1373</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>71</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>1373</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>72</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>73</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>1364</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>74</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -9743,21 +9743,21 @@
         <v>75</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1427</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>76</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -9765,10 +9765,10 @@
         <v>77</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>1377</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -9776,142 +9776,142 @@
         <v>78</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1427</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>79</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>80</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>1365</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>81</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>1368</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>82</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>1368</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>83</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>1366</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>84</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>1366</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>85</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>1378</v>
+        <v>1375</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>86</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>87</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>88</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>1367</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>89</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>1373</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>90</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>1379</v>
+        <v>1376</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>1373</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -9919,10 +9919,10 @@
         <v>91</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>1377</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -9930,10 +9930,10 @@
         <v>92</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>1377</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -9941,10 +9941,10 @@
         <v>93</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>1380</v>
+        <v>1377</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>1377</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -9952,10 +9952,10 @@
         <v>94</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>1377</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -9963,24 +9963,24 @@
         <v>95</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>1357</v>
+        <v>1426</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1427</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>971</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>1358</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1356</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>972</v>
       </c>
@@ -9991,41 +9991,47 @@
         <v>100</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>973</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>1359</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>974</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>1360</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>976</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1" xr:uid="{8396C999-8A46-4619-A745-8444C9CAECCE}"/>
+  <autoFilter ref="A1:C102" xr:uid="{8396C999-8A46-4619-A745-8444C9CAECCE}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Ile-de-France"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -10072,7 +10078,7 @@
   <sheetData>
     <row r="1" spans="1:69" ht="13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>1391</v>
+        <v>1388</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>225</v>
@@ -48326,154 +48332,154 @@
   <sheetData>
     <row r="1" spans="1:7" ht="13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>1392</v>
+        <v>1389</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1408</v>
+        <v>1405</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1410</v>
+        <v>1407</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1409</v>
+        <v>1406</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>1414</v>
+        <v>1411</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>1415</v>
+        <v>1412</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>1416</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1394</v>
+        <v>1391</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>1406</v>
+        <v>1403</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1412</v>
+        <v>1409</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>1412</v>
+        <v>1409</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>1413</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1396</v>
+        <v>1393</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>1406</v>
+        <v>1403</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>1412</v>
+        <v>1409</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>1412</v>
+        <v>1409</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>1413</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>1397</v>
+        <v>1394</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>1406</v>
+        <v>1403</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>1412</v>
+        <v>1409</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>1412</v>
+        <v>1409</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>1413</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>1398</v>
+        <v>1395</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>1406</v>
+        <v>1403</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>1412</v>
+        <v>1409</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>1412</v>
+        <v>1409</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>1413</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>1399</v>
+        <v>1396</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>1406</v>
+        <v>1403</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>1407</v>
+        <v>1404</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>1413</v>
+        <v>1410</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>1413</v>
+        <v>1410</v>
       </c>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>1400</v>
+        <v>1397</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>1406</v>
+        <v>1403</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>1407</v>
+        <v>1404</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>1413</v>
+        <v>1410</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>1413</v>
+        <v>1410</v>
       </c>
       <c r="G7" s="4"/>
     </row>
@@ -48491,9 +48497,9 @@
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -48507,299 +48513,299 @@
   <sheetData>
     <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>1392</v>
+        <v>1389</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1393</v>
+        <v>1390</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>1405</v>
+        <v>1402</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1403</v>
+        <v>1400</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>1411</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1394</v>
+        <v>1391</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
       <c r="C2" s="9">
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>1412</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1396</v>
+        <v>1393</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
       <c r="C3" s="9">
         <v>4</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>1412</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>1397</v>
+        <v>1394</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
       <c r="C4" s="9">
         <v>3</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>1412</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>1398</v>
+        <v>1395</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
       <c r="C5" s="9">
         <v>2</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>1412</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>1399</v>
+        <v>1396</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
       <c r="C6" s="9">
         <v>5</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>1406</v>
+        <v>1403</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>1413</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>1400</v>
+        <v>1397</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
       <c r="C7" s="9">
         <v>6</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>1406</v>
+        <v>1403</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>1413</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>1394</v>
+        <v>1391</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>1398</v>
+      </c>
+      <c r="C8" s="9">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>1401</v>
       </c>
-      <c r="C8" s="9">
-        <v>1</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>1404</v>
-      </c>
       <c r="E8" s="11" t="s">
-        <v>1426</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>1396</v>
+        <v>1393</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>1401</v>
+        <v>1398</v>
       </c>
       <c r="C9" s="9">
         <v>4</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>1426</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>1397</v>
+        <v>1394</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>1401</v>
+        <v>1398</v>
       </c>
       <c r="C10" s="9">
         <v>3</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>1426</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>1395</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>1398</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>1401</v>
       </c>
       <c r="C11" s="9">
         <v>2</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>1426</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>1399</v>
+        <v>1396</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>1401</v>
+        <v>1398</v>
       </c>
       <c r="C12" s="9">
         <v>5</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>1407</v>
+        <v>1404</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>1427</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>1400</v>
+        <v>1397</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>1401</v>
+        <v>1398</v>
       </c>
       <c r="C13" s="9">
         <v>6</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>1407</v>
+        <v>1404</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>1427</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>1394</v>
+        <v>1391</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
       <c r="C14" s="9">
         <v>1</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>1406</v>
+        <v>1403</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>1427</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>1396</v>
+        <v>1393</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
       <c r="C15" s="9">
         <v>4</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>1406</v>
+        <v>1403</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>1427</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>1397</v>
+        <v>1394</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
       <c r="C16" s="9">
         <v>3</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>1406</v>
+        <v>1403</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>1427</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>1398</v>
+        <v>1395</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
       <c r="C17" s="9">
         <v>2</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>1406</v>
+        <v>1403</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>1427</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>1399</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>1402</v>
       </c>
       <c r="C18" s="9">
         <v>5</v>
@@ -48809,10 +48815,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>1400</v>
+        <v>1397</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
       <c r="C19" s="9">
         <v>6</v>
@@ -48847,15 +48853,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>1417</v>
+        <v>1414</v>
       </c>
       <c r="B2" s="4">
         <v>0</v>
@@ -48919,7 +48925,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>1418</v>
+        <v>1415</v>
       </c>
       <c r="B10" s="4">
         <v>8</v>

</xml_diff>

<commit_message>
feat: add sheet parameters for maps
</commit_message>
<xml_diff>
--- a/data_input/REF_WSR.xlsx
+++ b/data_input/REF_WSR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flore\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8B976C-43C4-4D07-B4B3-B7D692A18003}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DDF358A-4D56-4A5B-925A-C700FF8C6FA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA_INPUT" sheetId="9" r:id="rId1"/>
@@ -21,8 +21,10 @@
     <sheet name="PARAM_ALL" sheetId="7" r:id="rId6"/>
     <sheet name="PARAM_TREND" sheetId="5" r:id="rId7"/>
     <sheet name="PARAM_ENTITIES" sheetId="8" r:id="rId8"/>
+    <sheet name="MAP_FRANCE" sheetId="12" r:id="rId9"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">MAP_FRANCE!$A$1:$Q$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">PARAM_ALL!$A$1:$G$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">PARAM_ENTITIES!$A$1:$B$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">PARAM_TREND!$A$1:$E$1</definedName>
@@ -46,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8500" uniqueCount="1483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8540" uniqueCount="1515">
   <si>
     <t>COUNTRY_REGION</t>
   </si>
@@ -4495,6 +4497,102 @@
   </si>
   <si>
     <t>São Tomé and Principe</t>
+  </si>
+  <si>
+    <t>FILE_HTML</t>
+  </si>
+  <si>
+    <t>DF_KEY</t>
+  </si>
+  <si>
+    <t>GEO_KEY</t>
+  </si>
+  <si>
+    <t>TO_RENAME</t>
+  </si>
+  <si>
+    <t>Hospitalisations</t>
+  </si>
+  <si>
+    <t>France_HOSP_DEP_NAME.html</t>
+  </si>
+  <si>
+    <t>LABEL</t>
+  </si>
+  <si>
+    <t>properties.nom</t>
+  </si>
+  <si>
+    <t>SCALE_MIN</t>
+  </si>
+  <si>
+    <t>SCALE_MAX</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>3000</t>
+  </si>
+  <si>
+    <t>#FFFFFF</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>0.05</t>
+  </si>
+  <si>
+    <t>#B3D7D2</t>
+  </si>
+  <si>
+    <t>0.10</t>
+  </si>
+  <si>
+    <t>0.55</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>#00354E</t>
+  </si>
+  <si>
+    <t>#437F9D</t>
+  </si>
+  <si>
+    <t>#81B1BD</t>
+  </si>
+  <si>
+    <t>COLORS_C1</t>
+  </si>
+  <si>
+    <t>COLORS_S1</t>
+  </si>
+  <si>
+    <t>COLORS_S2</t>
+  </si>
+  <si>
+    <t>COLORS_C2</t>
+  </si>
+  <si>
+    <t>COLORS_C5</t>
+  </si>
+  <si>
+    <t>COLORS_S5</t>
+  </si>
+  <si>
+    <t>COLORS_C4</t>
+  </si>
+  <si>
+    <t>COLORS_S4</t>
+  </si>
+  <si>
+    <t>COLORS_C3</t>
+  </si>
+  <si>
+    <t>COLORS_S3</t>
   </si>
 </sst>
 </file>
@@ -5036,7 +5134,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5067,6 +5165,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5430,7 +5549,7 @@
   <dimension ref="A1:F187"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5480,9 +5599,15 @@
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="A3" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" s="5">
+        <v>20200519</v>
+      </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -6970,14 +7095,14 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:E190"/>
+  <dimension ref="A1:E191"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B112" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B185" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B11" sqref="B11"/>
       <selection pane="topRight" activeCell="B11" sqref="B11"/>
       <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
-      <selection pane="bottomRight" activeCell="F121" sqref="F121"/>
+      <selection pane="bottomRight" activeCell="D196" sqref="D196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -10548,6 +10673,23 @@
         <v>222</v>
       </c>
       <c r="E190" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B191" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C191" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="D191" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="E191" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -48831,12 +48973,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9113378-5D39-4843-B996-FB70A65D1BC4}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:C233"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B150" sqref="B150"/>
+      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -48855,7 +48996,7 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1432</v>
       </c>
@@ -48866,7 +49007,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1433</v>
       </c>
@@ -48877,7 +49018,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1434</v>
       </c>
@@ -48888,7 +49029,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>170</v>
       </c>
@@ -48899,7 +49040,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>1435</v>
       </c>
@@ -48910,7 +49051,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>179</v>
       </c>
@@ -48921,7 +49062,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>1436</v>
       </c>
@@ -48932,7 +49073,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -48943,7 +49084,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>34</v>
       </c>
@@ -48954,7 +49095,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>42</v>
       </c>
@@ -48965,7 +49106,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>46</v>
       </c>
@@ -48976,7 +49117,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>1437</v>
       </c>
@@ -48987,7 +49128,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>1438</v>
       </c>
@@ -48998,7 +49139,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>174</v>
       </c>
@@ -49009,7 +49150,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>195</v>
       </c>
@@ -49020,7 +49161,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>175</v>
       </c>
@@ -49031,7 +49172,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>68</v>
       </c>
@@ -49042,7 +49183,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>199</v>
       </c>
@@ -49053,7 +49194,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>72</v>
       </c>
@@ -49064,7 +49205,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>82</v>
       </c>
@@ -49075,7 +49216,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>164</v>
       </c>
@@ -49086,7 +49227,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>1439</v>
       </c>
@@ -49097,7 +49238,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>129</v>
       </c>
@@ -49108,7 +49249,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>1440</v>
       </c>
@@ -49119,7 +49260,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>1441</v>
       </c>
@@ -49130,7 +49271,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>103</v>
       </c>
@@ -49141,7 +49282,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>113</v>
       </c>
@@ -49152,7 +49293,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>119</v>
       </c>
@@ -49163,7 +49304,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>208</v>
       </c>
@@ -49174,7 +49315,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>54</v>
       </c>
@@ -49185,7 +49326,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>1442</v>
       </c>
@@ -49196,7 +49337,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>1443</v>
       </c>
@@ -49207,7 +49348,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>1444</v>
       </c>
@@ -49218,7 +49359,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>151</v>
       </c>
@@ -49229,7 +49370,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>220</v>
       </c>
@@ -49240,7 +49381,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>1445</v>
       </c>
@@ -49251,7 +49392,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>1446</v>
       </c>
@@ -49262,7 +49403,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>1447</v>
       </c>
@@ -49273,7 +49414,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>11</v>
       </c>
@@ -49284,7 +49425,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>26</v>
       </c>
@@ -49295,7 +49436,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>28</v>
       </c>
@@ -49306,7 +49447,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>37</v>
       </c>
@@ -49317,7 +49458,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>39</v>
       </c>
@@ -49328,7 +49469,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>52</v>
       </c>
@@ -49339,7 +49480,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>196</v>
       </c>
@@ -49350,7 +49491,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>70</v>
       </c>
@@ -49361,7 +49502,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>121</v>
       </c>
@@ -49372,7 +49513,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>120</v>
       </c>
@@ -49383,7 +49524,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>144</v>
       </c>
@@ -49394,7 +49535,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>2</v>
       </c>
@@ -49405,7 +49546,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>157</v>
       </c>
@@ -49416,7 +49557,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>160</v>
       </c>
@@ -49427,7 +49568,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>155</v>
       </c>
@@ -49438,7 +49579,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>13</v>
       </c>
@@ -49449,7 +49590,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>17</v>
       </c>
@@ -49460,7 +49601,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>20</v>
       </c>
@@ -49471,7 +49612,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>19</v>
       </c>
@@ -49482,7 +49623,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>29</v>
       </c>
@@ -49493,7 +49634,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>25</v>
       </c>
@@ -49504,7 +49645,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>38</v>
       </c>
@@ -49515,7 +49656,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>193</v>
       </c>
@@ -49526,7 +49667,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>47</v>
       </c>
@@ -49537,7 +49678,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="64" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>64</v>
       </c>
@@ -49548,7 +49689,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>1448</v>
       </c>
@@ -49559,7 +49700,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="66" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>1449</v>
       </c>
@@ -49570,7 +49711,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>76</v>
       </c>
@@ -49581,7 +49722,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>75</v>
       </c>
@@ -49592,7 +49733,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>77</v>
       </c>
@@ -49603,7 +49744,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>78</v>
       </c>
@@ -49614,7 +49755,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="71" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>84</v>
       </c>
@@ -49625,7 +49766,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>80</v>
       </c>
@@ -49636,7 +49777,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>83</v>
       </c>
@@ -49647,7 +49788,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>1450</v>
       </c>
@@ -49658,7 +49799,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>85</v>
       </c>
@@ -49669,7 +49810,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>90</v>
       </c>
@@ -49680,7 +49821,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="77" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>32</v>
       </c>
@@ -49691,7 +49832,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>200</v>
       </c>
@@ -49702,7 +49843,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="79" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>89</v>
       </c>
@@ -49713,7 +49854,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="80" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>201</v>
       </c>
@@ -49724,7 +49865,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>92</v>
       </c>
@@ -49735,7 +49876,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="82" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>142</v>
       </c>
@@ -49746,7 +49887,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="83" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>1451</v>
       </c>
@@ -49757,7 +49898,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="84" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>205</v>
       </c>
@@ -49768,7 +49909,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="85" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>106</v>
       </c>
@@ -49779,7 +49920,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="86" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>97</v>
       </c>
@@ -49790,7 +49931,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="87" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>110</v>
       </c>
@@ -49801,7 +49942,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="88" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>117</v>
       </c>
@@ -49812,7 +49953,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="89" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>118</v>
       </c>
@@ -49823,7 +49964,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="90" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>122</v>
       </c>
@@ -49834,7 +49975,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="91" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>209</v>
       </c>
@@ -49845,7 +49986,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="92" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>210</v>
       </c>
@@ -49856,7 +49997,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="93" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>125</v>
       </c>
@@ -49867,7 +50008,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="94" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>132</v>
       </c>
@@ -49878,7 +50019,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="95" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>136</v>
       </c>
@@ -49889,7 +50030,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="96" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>177</v>
       </c>
@@ -49900,7 +50041,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>149</v>
       </c>
@@ -49911,7 +50052,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>217</v>
       </c>
@@ -49922,7 +50063,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>218</v>
       </c>
@@ -49933,7 +50074,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>178</v>
       </c>
@@ -49944,7 +50085,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>153</v>
       </c>
@@ -49955,7 +50096,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>219</v>
       </c>
@@ -49966,7 +50107,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="103" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>159</v>
       </c>
@@ -49977,7 +50118,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="104" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>161</v>
       </c>
@@ -49988,7 +50129,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>165</v>
       </c>
@@ -49999,7 +50140,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>186</v>
       </c>
@@ -50010,7 +50151,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="107" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>222</v>
       </c>
@@ -50021,7 +50162,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>24</v>
       </c>
@@ -50032,7 +50173,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>31</v>
       </c>
@@ -50043,7 +50184,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>188</v>
       </c>
@@ -50054,7 +50195,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>189</v>
       </c>
@@ -50065,7 +50206,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>1452</v>
       </c>
@@ -50076,7 +50217,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="113" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>33</v>
       </c>
@@ -50087,7 +50228,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="114" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>191</v>
       </c>
@@ -50098,7 +50239,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="115" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>192</v>
       </c>
@@ -50109,7 +50250,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="116" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>1453</v>
       </c>
@@ -50120,7 +50261,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="117" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>1454</v>
       </c>
@@ -50131,7 +50272,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="118" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>50</v>
       </c>
@@ -50142,7 +50283,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="119" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>6</v>
       </c>
@@ -50153,7 +50294,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="120" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>53</v>
       </c>
@@ -50164,7 +50305,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="121" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>171</v>
       </c>
@@ -50175,7 +50316,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="122" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>58</v>
       </c>
@@ -50186,7 +50327,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="123" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>62</v>
       </c>
@@ -50197,7 +50338,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="124" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>66</v>
       </c>
@@ -50208,7 +50349,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="125" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>69</v>
       </c>
@@ -50219,7 +50360,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="126" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>172</v>
       </c>
@@ -50230,7 +50371,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="127" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>197</v>
       </c>
@@ -50241,7 +50382,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="128" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>198</v>
       </c>
@@ -50252,7 +50393,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="129" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>86</v>
       </c>
@@ -50263,7 +50404,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="130" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>93</v>
       </c>
@@ -50274,7 +50415,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="131" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>181</v>
       </c>
@@ -50285,7 +50426,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="132" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>202</v>
       </c>
@@ -50296,7 +50437,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="133" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>108</v>
       </c>
@@ -50307,7 +50448,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="134" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>163</v>
       </c>
@@ -50318,7 +50459,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="135" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>204</v>
       </c>
@@ -50329,7 +50470,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="136" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>176</v>
       </c>
@@ -50340,7 +50481,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="137" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>101</v>
       </c>
@@ -50351,7 +50492,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="138" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>206</v>
       </c>
@@ -50362,7 +50503,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="139" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>109</v>
       </c>
@@ -50373,7 +50514,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="140" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>167</v>
       </c>
@@ -50384,7 +50525,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="141" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>114</v>
       </c>
@@ -50395,7 +50536,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="142" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>128</v>
       </c>
@@ -50406,7 +50547,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="143" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>211</v>
       </c>
@@ -50417,7 +50558,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="144" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>212</v>
       </c>
@@ -50428,7 +50569,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="145" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>143</v>
       </c>
@@ -50439,7 +50580,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="146" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>133</v>
       </c>
@@ -50450,7 +50591,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="147" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>214</v>
       </c>
@@ -50461,7 +50602,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="148" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>215</v>
       </c>
@@ -50472,7 +50613,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="149" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>139</v>
       </c>
@@ -50494,7 +50635,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="151" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>216</v>
       </c>
@@ -50505,7 +50646,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="152" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>36</v>
       </c>
@@ -50516,7 +50657,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="153" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>150</v>
       </c>
@@ -50527,7 +50668,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="154" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>152</v>
       </c>
@@ -50538,7 +50679,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="155" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>148</v>
       </c>
@@ -50549,7 +50690,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="156" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>173</v>
       </c>
@@ -50560,7 +50701,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="157" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>140</v>
       </c>
@@ -50571,7 +50712,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="158" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>162</v>
       </c>
@@ -50582,7 +50723,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="159" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>169</v>
       </c>
@@ -50593,7 +50734,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="160" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>4</v>
       </c>
@@ -50604,7 +50745,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="161" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>1456</v>
       </c>
@@ -50615,7 +50756,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="162" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>8</v>
       </c>
@@ -50626,7 +50767,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="163" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>16</v>
       </c>
@@ -50637,7 +50778,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="164" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>23</v>
       </c>
@@ -50648,7 +50789,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="165" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>30</v>
       </c>
@@ -50659,7 +50800,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="166" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>187</v>
       </c>
@@ -50670,7 +50811,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="167" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>22</v>
       </c>
@@ -50681,7 +50822,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="168" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>146</v>
       </c>
@@ -50692,7 +50833,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="169" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>194</v>
       </c>
@@ -50703,7 +50844,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="170" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>65</v>
       </c>
@@ -50714,7 +50855,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="171" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>49</v>
       </c>
@@ -50725,7 +50866,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="172" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>141</v>
       </c>
@@ -50736,7 +50877,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="173" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>56</v>
       </c>
@@ -50747,7 +50888,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="174" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>60</v>
       </c>
@@ -50758,7 +50899,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="175" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>61</v>
       </c>
@@ -50769,7 +50910,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="176" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>1457</v>
       </c>
@@ -50780,7 +50921,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="177" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>156</v>
       </c>
@@ -50791,7 +50932,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="178" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>1458</v>
       </c>
@@ -50802,7 +50943,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="179" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>67</v>
       </c>
@@ -50813,7 +50954,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="180" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>44</v>
       </c>
@@ -50824,7 +50965,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="181" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>73</v>
       </c>
@@ -50835,7 +50976,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="182" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>1459</v>
       </c>
@@ -50846,7 +50987,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="183" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>79</v>
       </c>
@@ -50857,7 +50998,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="184" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>74</v>
       </c>
@@ -50868,7 +51009,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="185" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>81</v>
       </c>
@@ -50879,7 +51020,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="186" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>1460</v>
       </c>
@@ -50890,7 +51031,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="187" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>88</v>
       </c>
@@ -50901,7 +51042,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="188" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>94</v>
       </c>
@@ -50912,7 +51053,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="189" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>95</v>
       </c>
@@ -50923,7 +51064,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="190" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>96</v>
       </c>
@@ -50934,7 +51075,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="191" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>91</v>
       </c>
@@ -50945,7 +51086,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="192" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>105</v>
       </c>
@@ -50956,7 +51097,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="193" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>104</v>
       </c>
@@ -50967,7 +51108,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="194" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>203</v>
       </c>
@@ -50978,7 +51119,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="195" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>99</v>
       </c>
@@ -50989,7 +51130,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="196" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>107</v>
       </c>
@@ -51000,7 +51141,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="197" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>111</v>
       </c>
@@ -51011,7 +51152,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="198" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>116</v>
       </c>
@@ -51022,7 +51163,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="199" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>123</v>
       </c>
@@ -51033,7 +51174,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="200" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>124</v>
       </c>
@@ -51044,7 +51185,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="201" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>126</v>
       </c>
@@ -51055,7 +51196,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="202" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>127</v>
       </c>
@@ -51066,7 +51207,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="203" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>131</v>
       </c>
@@ -51077,7 +51218,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="204" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>134</v>
       </c>
@@ -51088,7 +51229,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="205" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>137</v>
       </c>
@@ -51099,7 +51240,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="206" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>138</v>
       </c>
@@ -51110,7 +51251,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="207" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>145</v>
       </c>
@@ -51121,7 +51262,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="208" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>154</v>
       </c>
@@ -51132,7 +51273,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="209" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>1461</v>
       </c>
@@ -51143,7 +51284,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="210" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>1462</v>
       </c>
@@ -51154,7 +51295,7 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="211" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>1464</v>
       </c>
@@ -51165,7 +51306,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="212" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>14</v>
       </c>
@@ -51176,7 +51317,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="213" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>1465</v>
       </c>
@@ -51187,7 +51328,7 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="214" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>59</v>
       </c>
@@ -51198,7 +51339,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="215" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>1466</v>
       </c>
@@ -51209,7 +51350,7 @@
         <v>1466</v>
       </c>
     </row>
-    <row r="216" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>1467</v>
       </c>
@@ -51220,7 +51361,7 @@
         <v>1466</v>
       </c>
     </row>
-    <row r="217" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>1468</v>
       </c>
@@ -51231,7 +51372,7 @@
         <v>1466</v>
       </c>
     </row>
-    <row r="218" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>1469</v>
       </c>
@@ -51242,7 +51383,7 @@
         <v>1466</v>
       </c>
     </row>
-    <row r="219" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>1470</v>
       </c>
@@ -51253,7 +51394,7 @@
         <v>1466</v>
       </c>
     </row>
-    <row r="220" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>207</v>
       </c>
@@ -51264,7 +51405,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="221" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>1471</v>
       </c>
@@ -51275,7 +51416,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="222" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>1472</v>
       </c>
@@ -51286,7 +51427,7 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="223" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>1473</v>
       </c>
@@ -51297,7 +51438,7 @@
         <v>1466</v>
       </c>
     </row>
-    <row r="224" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>1474</v>
       </c>
@@ -51308,7 +51449,7 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="225" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>112</v>
       </c>
@@ -51319,7 +51460,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="226" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>1475</v>
       </c>
@@ -51330,7 +51471,7 @@
         <v>1466</v>
       </c>
     </row>
-    <row r="227" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>168</v>
       </c>
@@ -51341,7 +51482,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="228" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>1476</v>
       </c>
@@ -51352,7 +51493,7 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="229" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>213</v>
       </c>
@@ -51363,7 +51504,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="230" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>1477</v>
       </c>
@@ -51374,7 +51515,7 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="231" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>221</v>
       </c>
@@ -51385,7 +51526,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="232" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>1478</v>
       </c>
@@ -51396,7 +51537,7 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="233" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>1479</v>
       </c>
@@ -51408,13 +51549,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C233" xr:uid="{F212CD21-2C9A-4C83-8A8A-3B26A918ACDA}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Sà£o Tomé and Principe"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:C233" xr:uid="{F212CD21-2C9A-4C83-8A8A-3B26A918ACDA}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -53102,7 +53237,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -53200,4 +53335,293 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{010FA2AE-1E3D-49FF-AFC3-96B6E33E47ED}">
+  <sheetPr>
+    <tabColor theme="0" tint="-0.14999847407452621"/>
+  </sheetPr>
+  <dimension ref="A1:Q10"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.6328125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.7265625" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.81640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="17" width="16.7265625" style="20" customWidth="1"/>
+    <col min="18" max="16384" width="10.90625" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="13" x14ac:dyDescent="0.35">
+      <c r="A1" s="14" t="s">
+        <v>1389</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>1484</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>1485</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>1486</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>1491</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>1492</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>1506</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>1505</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>1507</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>1508</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>1514</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>1513</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>1512</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>1511</v>
+      </c>
+      <c r="P1" s="14" t="s">
+        <v>1510</v>
+      </c>
+      <c r="Q1" s="14" t="s">
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="25" x14ac:dyDescent="0.35">
+      <c r="A2" s="16" t="s">
+        <v>1487</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>1488</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>1489</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>1490</v>
+      </c>
+      <c r="E2" s="18" t="str">
+        <f>"{'LABEL': 'Département','VALUE': '"&amp;A2&amp;"', 'VAR': 'Variation en nb.'}"</f>
+        <v>{'LABEL': 'Département','VALUE': 'Hospitalisations', 'VAR': 'Variation en nb.'}</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>1493</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>1494</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>1496</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>1495</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>1497</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>1498</v>
+      </c>
+      <c r="L2" s="19" t="s">
+        <v>1499</v>
+      </c>
+      <c r="M2" s="19" t="s">
+        <v>1504</v>
+      </c>
+      <c r="N2" s="19" t="s">
+        <v>1500</v>
+      </c>
+      <c r="O2" s="19" t="s">
+        <v>1503</v>
+      </c>
+      <c r="P2" s="19" t="s">
+        <v>1501</v>
+      </c>
+      <c r="Q2" s="19" t="s">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" s="16"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6" s="16"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" s="16"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8" s="16"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9" s="16"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10" s="16"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:Q1" xr:uid="{2FB4E092-F6B6-426F-AB87-3FE12C5A15C5}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>